<commit_message>
temp dropping of datatable
</commit_message>
<xml_diff>
--- a/oxshef-viz-tutorials-etc.xlsx
+++ b/oxshef-viz-tutorials-etc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martinjhnhadley/Github/oxshef_charts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02CB66A7-644B-2945-8143-AC4FE66B2483}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60772ECB-B981-6C48-87DD-25578FD861B4}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25600" yWindow="460" windowWidth="25600" windowHeight="27380" xr2:uid="{9D0B70CF-CB63-3344-B41D-6EFEDEBDA8D7}"/>
   </bookViews>
@@ -491,7 +491,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>